<commit_message>
Modify excel sheets categories structure
</commit_message>
<xml_diff>
--- a/data_and_results/monthly data/2099.01.xlsx
+++ b/data_and_results/monthly data/2099.01.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20736" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="01" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="B11" authorId="0">
+    <comment ref="B11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="0">
+    <comment ref="C11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D11" authorId="0">
+    <comment ref="D11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -96,7 +96,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E11" authorId="0">
+    <comment ref="E11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -120,7 +120,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="0">
+    <comment ref="F11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -144,7 +144,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G11" authorId="0">
+    <comment ref="G11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -168,7 +168,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H11" authorId="0">
+    <comment ref="H11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -192,7 +192,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I11" authorId="0">
+    <comment ref="I11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -216,7 +216,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M11" authorId="0">
+    <comment ref="N11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -240,7 +240,271 @@
         </r>
       </text>
     </comment>
-    <comment ref="P11" authorId="0">
+    <comment ref="B12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+masarnia</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+media</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+perfumy</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+przejazdy</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+spotify</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+basen</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+obiady</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+dezodorant</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+uber</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+wyjście na piwo</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+piekarnia</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -264,271 +528,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Autor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-masarnia</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C12" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Autor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-media</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D12" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Autor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-perfumy</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F12" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Autor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-przejazdy</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G12" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Autor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-spotify</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H12" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Autor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-basen</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B13" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Autor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-obiady</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D13" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Autor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-dezodorant</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F13" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Autor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-uber</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H13" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Autor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-wyjście na piwo</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B14" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Autor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-piekarnia</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B15" authorId="0">
+    <comment ref="B15" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -552,7 +552,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B16" authorId="0">
+    <comment ref="B16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -576,7 +576,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B17" authorId="0">
+    <comment ref="B17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -605,7 +605,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Jedzenie</t>
   </si>
@@ -643,9 +643,6 @@
     <t>Przychody:</t>
   </si>
   <si>
-    <t>Papiernicze i biurowe</t>
-  </si>
-  <si>
     <t>Procent [%]</t>
   </si>
   <si>
@@ -659,9 +656,6 @@
   </si>
   <si>
     <t>Transport i noclegi</t>
-  </si>
-  <si>
-    <t>Kultura</t>
   </si>
   <si>
     <t>Prez/don:</t>
@@ -691,8 +685,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1372,43 +1366,43 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.75" thickBot="1">
+    <row r="1" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" s="31">
         <f>E1-A9</f>
@@ -1433,9 +1427,9 @@
       <c r="K1" s="19"/>
       <c r="L1" s="20"/>
     </row>
-    <row r="2" spans="1:27" ht="15.75" thickBot="1">
+    <row r="2" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="32">
         <f>E2-A9</f>
@@ -1443,7 +1437,7 @@
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="10">
         <f>SUM(F2:K2)</f>
@@ -1476,15 +1470,15 @@
       <c r="Z2" s="4"/>
       <c r="AA2" s="4"/>
     </row>
-    <row r="3" spans="1:27" ht="15.75" thickBot="1">
+    <row r="3" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E3" s="30" t="s">
         <v>4</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H3" s="23"/>
       <c r="I3" s="23"/>
@@ -1507,7 +1501,7 @@
       <c r="Z3" s="4"/>
       <c r="AA3" s="4"/>
     </row>
-    <row r="4" spans="1:27" ht="15.75" thickBot="1">
+    <row r="4" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="4"/>
@@ -1532,18 +1526,18 @@
       <c r="Z4" s="4"/>
       <c r="AA4" s="4"/>
     </row>
-    <row r="5" spans="1:27">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
@@ -1569,18 +1563,18 @@
       <c r="Z5" s="4"/>
       <c r="AA5" s="4"/>
     </row>
-    <row r="6" spans="1:27" ht="15.75" thickBot="1">
+    <row r="6" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="28">
         <f>SUM(B9+C9+D9+F9+E9+G9)</f>
         <v>1905.5</v>
       </c>
       <c r="B6" s="29">
         <f>SUM(H9+J9+K9+I9+L9+N9+P9+O9)</f>
-        <v>499</v>
+        <v>519</v>
       </c>
       <c r="C6" s="29">
         <f>SUM(M9)</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D6" s="33">
         <v>1000</v>
@@ -1609,7 +1603,7 @@
       <c r="Z6" s="4"/>
       <c r="AA6" s="4"/>
     </row>
-    <row r="7" spans="1:27" ht="15.75" thickBot="1">
+    <row r="7" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1625,9 +1619,9 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="1:27" ht="15.75" thickBot="1">
+    <row r="8" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="6">
         <f t="shared" ref="B8:T8" si="0">100*B9/$A$9</f>
@@ -1655,7 +1649,7 @@
       </c>
       <c r="H8" s="6">
         <f t="shared" si="1"/>
-        <v>5.1144565889874203</v>
+        <v>6.1455970303155292</v>
       </c>
       <c r="I8" s="6">
         <f t="shared" si="1"/>
@@ -1675,11 +1669,11 @@
       </c>
       <c r="M8" s="6">
         <f t="shared" ref="M8:S8" si="2">100*M9/$A$9</f>
-        <v>0.82491235306248711</v>
+        <v>0</v>
       </c>
       <c r="N8" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.82491235306248711</v>
       </c>
       <c r="O8" s="6">
         <f t="shared" si="2"/>
@@ -1687,7 +1681,7 @@
       </c>
       <c r="P8" s="6">
         <f t="shared" si="2"/>
-        <v>1.0311404413281089</v>
+        <v>0</v>
       </c>
       <c r="Q8" s="6">
         <f t="shared" si="2"/>
@@ -1706,7 +1700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="15.75" thickBot="1">
+    <row r="9" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <f>SUM(B9:Z9)</f>
         <v>2424.5</v>
@@ -1737,7 +1731,7 @@
       </c>
       <c r="H9" s="16">
         <f t="shared" si="3"/>
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="I9" s="16">
         <f t="shared" si="3"/>
@@ -1756,20 +1750,20 @@
         <v>0</v>
       </c>
       <c r="M9" s="16">
-        <f t="shared" si="3"/>
+        <f>SUM(M12:M706)</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="16">
+        <f>SUM(N11:N706)</f>
         <v>20</v>
       </c>
-      <c r="N9" s="16">
+      <c r="O9" s="16">
+        <f>SUM(O12:O706)</f>
+        <v>0</v>
+      </c>
+      <c r="P9" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
-      </c>
-      <c r="O9" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P9" s="16">
-        <f t="shared" si="3"/>
-        <v>25</v>
       </c>
       <c r="Q9" s="16">
         <f t="shared" si="3"/>
@@ -1788,7 +1782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>4</v>
       </c>
@@ -1805,7 +1799,7 @@
         <v>6</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G10" s="14" t="s">
         <v>5</v>
@@ -1814,7 +1808,7 @@
         <v>1</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J10" s="14" t="s">
         <v>2</v>
@@ -1826,23 +1820,19 @@
         <v>7</v>
       </c>
       <c r="M10" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="N10" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="N10" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="O10" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="P10" s="24" t="s">
-        <v>18</v>
-      </c>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
       <c r="Q10" s="24"/>
       <c r="R10" s="24"/>
       <c r="S10" s="24"/>
       <c r="T10" s="24"/>
     </row>
-    <row r="11" spans="1:27">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>1</v>
       </c>
@@ -1873,20 +1863,18 @@
       <c r="J11" s="19"/>
       <c r="K11" s="19"/>
       <c r="L11" s="19"/>
-      <c r="M11" s="19">
+      <c r="M11" s="19"/>
+      <c r="N11" s="19">
         <v>20</v>
       </c>
-      <c r="N11" s="19"/>
       <c r="O11" s="19"/>
-      <c r="P11" s="19">
-        <v>25</v>
-      </c>
+      <c r="P11" s="19"/>
       <c r="Q11" s="19"/>
       <c r="R11" s="19"/>
       <c r="S11" s="19"/>
       <c r="T11" s="19"/>
     </row>
-    <row r="12" spans="1:27">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>2</v>
       </c>
@@ -1922,7 +1910,7 @@
       <c r="S12" s="19"/>
       <c r="T12" s="19"/>
     </row>
-    <row r="13" spans="1:27">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>3</v>
       </c>
@@ -1954,7 +1942,7 @@
       <c r="S13" s="19"/>
       <c r="T13" s="19"/>
     </row>
-    <row r="14" spans="1:27">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" s="13">
         <v>4</v>
       </c>
@@ -1966,7 +1954,9 @@
       <c r="E14" s="19"/>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
+      <c r="H14" s="19">
+        <v>25</v>
+      </c>
       <c r="I14" s="19"/>
       <c r="J14" s="19"/>
       <c r="K14" s="19"/>
@@ -1980,7 +1970,7 @@
       <c r="S14" s="19"/>
       <c r="T14" s="19"/>
     </row>
-    <row r="15" spans="1:27">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" s="13">
         <v>5</v>
       </c>
@@ -2006,7 +1996,7 @@
       <c r="S15" s="19"/>
       <c r="T15" s="19"/>
     </row>
-    <row r="16" spans="1:27">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" s="13">
         <v>6</v>
       </c>
@@ -2032,7 +2022,7 @@
       <c r="S16" s="19"/>
       <c r="T16" s="19"/>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="13">
         <v>7</v>
       </c>
@@ -2058,7 +2048,7 @@
       <c r="S17" s="19"/>
       <c r="T17" s="19"/>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="13">
         <v>8</v>
       </c>
@@ -2082,7 +2072,7 @@
       <c r="S18" s="19"/>
       <c r="T18" s="19"/>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="13">
         <v>9</v>
       </c>
@@ -2106,7 +2096,7 @@
       <c r="S19" s="19"/>
       <c r="T19" s="19"/>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="13">
         <v>10</v>
       </c>
@@ -2130,7 +2120,7 @@
       <c r="S20" s="19"/>
       <c r="T20" s="19"/>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="13">
         <v>11</v>
       </c>
@@ -2154,7 +2144,7 @@
       <c r="S21" s="19"/>
       <c r="T21" s="19"/>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="13">
         <v>12</v>
       </c>
@@ -2178,7 +2168,7 @@
       <c r="S22" s="19"/>
       <c r="T22" s="19"/>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="13">
         <v>13</v>
       </c>
@@ -2202,7 +2192,7 @@
       <c r="S23" s="19"/>
       <c r="T23" s="19"/>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="13">
         <v>14</v>
       </c>
@@ -2226,7 +2216,7 @@
       <c r="S24" s="19"/>
       <c r="T24" s="19"/>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="13">
         <v>15</v>
       </c>
@@ -2250,7 +2240,7 @@
       <c r="S25" s="19"/>
       <c r="T25" s="19"/>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="13">
         <v>16</v>
       </c>
@@ -2274,7 +2264,7 @@
       <c r="S26" s="19"/>
       <c r="T26" s="19"/>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="13">
         <v>17</v>
       </c>
@@ -2298,7 +2288,7 @@
       <c r="S27" s="19"/>
       <c r="T27" s="19"/>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="13">
         <v>18</v>
       </c>
@@ -2322,7 +2312,7 @@
       <c r="S28" s="19"/>
       <c r="T28" s="19"/>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="13">
         <v>19</v>
       </c>
@@ -2346,7 +2336,7 @@
       <c r="S29" s="19"/>
       <c r="T29" s="19"/>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" s="13">
         <v>20</v>
       </c>
@@ -2370,7 +2360,7 @@
       <c r="S30" s="19"/>
       <c r="T30" s="19"/>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" s="13">
         <v>21</v>
       </c>
@@ -2394,7 +2384,7 @@
       <c r="S31" s="19"/>
       <c r="T31" s="19"/>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="13">
         <v>22</v>
       </c>
@@ -2418,7 +2408,7 @@
       <c r="S32" s="19"/>
       <c r="T32" s="19"/>
     </row>
-    <row r="33" spans="1:20">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" s="13">
         <v>23</v>
       </c>
@@ -2442,7 +2432,7 @@
       <c r="S33" s="19"/>
       <c r="T33" s="19"/>
     </row>
-    <row r="34" spans="1:20">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" s="13">
         <v>24</v>
       </c>
@@ -2466,7 +2456,7 @@
       <c r="S34" s="19"/>
       <c r="T34" s="19"/>
     </row>
-    <row r="35" spans="1:20">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" s="13">
         <v>25</v>
       </c>
@@ -2490,7 +2480,7 @@
       <c r="S35" s="19"/>
       <c r="T35" s="19"/>
     </row>
-    <row r="36" spans="1:20">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" s="13">
         <v>26</v>
       </c>
@@ -2514,7 +2504,7 @@
       <c r="S36" s="19"/>
       <c r="T36" s="19"/>
     </row>
-    <row r="37" spans="1:20">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" s="13">
         <v>27</v>
       </c>
@@ -2538,7 +2528,7 @@
       <c r="S37" s="19"/>
       <c r="T37" s="19"/>
     </row>
-    <row r="38" spans="1:20">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" s="13">
         <v>28</v>
       </c>
@@ -2562,7 +2552,7 @@
       <c r="S38" s="19"/>
       <c r="T38" s="19"/>
     </row>
-    <row r="39" spans="1:20">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" s="13">
         <v>29</v>
       </c>
@@ -2586,7 +2576,7 @@
       <c r="S39" s="19"/>
       <c r="T39" s="19"/>
     </row>
-    <row r="40" spans="1:20">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" s="13">
         <v>30</v>
       </c>
@@ -2610,7 +2600,7 @@
       <c r="S40" s="19"/>
       <c r="T40" s="19"/>
     </row>
-    <row r="41" spans="1:20">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" s="13">
         <v>31</v>
       </c>
@@ -2634,7 +2624,7 @@
       <c r="S41" s="19"/>
       <c r="T41" s="19"/>
     </row>
-    <row r="42" spans="1:20">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" s="13">
         <v>32</v>
       </c>
@@ -2658,7 +2648,7 @@
       <c r="S42" s="19"/>
       <c r="T42" s="19"/>
     </row>
-    <row r="43" spans="1:20">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" s="13">
         <v>33</v>
       </c>
@@ -2682,7 +2672,7 @@
       <c r="S43" s="19"/>
       <c r="T43" s="19"/>
     </row>
-    <row r="44" spans="1:20">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44" s="13">
         <v>34</v>
       </c>
@@ -2706,7 +2696,7 @@
       <c r="S44" s="19"/>
       <c r="T44" s="19"/>
     </row>
-    <row r="45" spans="1:20">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" s="13">
         <v>35</v>
       </c>
@@ -2730,7 +2720,7 @@
       <c r="S45" s="19"/>
       <c r="T45" s="19"/>
     </row>
-    <row r="46" spans="1:20">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" s="13">
         <v>36</v>
       </c>
@@ -2754,7 +2744,7 @@
       <c r="S46" s="19"/>
       <c r="T46" s="19"/>
     </row>
-    <row r="47" spans="1:20">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" s="13">
         <v>37</v>
       </c>
@@ -2778,7 +2768,7 @@
       <c r="S47" s="19"/>
       <c r="T47" s="19"/>
     </row>
-    <row r="48" spans="1:20">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48" s="13">
         <v>38</v>
       </c>
@@ -2802,7 +2792,7 @@
       <c r="S48" s="19"/>
       <c r="T48" s="19"/>
     </row>
-    <row r="49" spans="1:20">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" s="13">
         <v>39</v>
       </c>
@@ -2826,7 +2816,7 @@
       <c r="S49" s="19"/>
       <c r="T49" s="19"/>
     </row>
-    <row r="50" spans="1:20">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" s="13">
         <v>40</v>
       </c>
@@ -2850,7 +2840,7 @@
       <c r="S50" s="19"/>
       <c r="T50" s="19"/>
     </row>
-    <row r="51" spans="1:20">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" s="13">
         <v>41</v>
       </c>
@@ -2874,7 +2864,7 @@
       <c r="S51" s="19"/>
       <c r="T51" s="19"/>
     </row>
-    <row r="52" spans="1:20">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52" s="13">
         <v>42</v>
       </c>
@@ -2898,7 +2888,7 @@
       <c r="S52" s="19"/>
       <c r="T52" s="19"/>
     </row>
-    <row r="53" spans="1:20">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53" s="13">
         <v>43</v>
       </c>
@@ -2922,7 +2912,7 @@
       <c r="S53" s="19"/>
       <c r="T53" s="19"/>
     </row>
-    <row r="54" spans="1:20">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54" s="13">
         <v>44</v>
       </c>
@@ -2946,7 +2936,7 @@
       <c r="S54" s="19"/>
       <c r="T54" s="19"/>
     </row>
-    <row r="55" spans="1:20">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55" s="13">
         <v>45</v>
       </c>
@@ -2970,7 +2960,7 @@
       <c r="S55" s="19"/>
       <c r="T55" s="19"/>
     </row>
-    <row r="56" spans="1:20">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56" s="13">
         <v>46</v>
       </c>
@@ -2994,7 +2984,7 @@
       <c r="S56" s="19"/>
       <c r="T56" s="19"/>
     </row>
-    <row r="57" spans="1:20">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" s="13">
         <v>47</v>
       </c>
@@ -3018,7 +3008,7 @@
       <c r="S57" s="19"/>
       <c r="T57" s="19"/>
     </row>
-    <row r="58" spans="1:20">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58" s="13">
         <v>48</v>
       </c>
@@ -3042,7 +3032,7 @@
       <c r="S58" s="19"/>
       <c r="T58" s="19"/>
     </row>
-    <row r="59" spans="1:20">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59" s="13">
         <v>49</v>
       </c>
@@ -3066,7 +3056,7 @@
       <c r="S59" s="19"/>
       <c r="T59" s="19"/>
     </row>
-    <row r="60" spans="1:20">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A60" s="13">
         <v>50</v>
       </c>
@@ -3090,7 +3080,7 @@
       <c r="S60" s="19"/>
       <c r="T60" s="19"/>
     </row>
-    <row r="61" spans="1:20">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A61" s="13">
         <v>51</v>
       </c>
@@ -3114,7 +3104,7 @@
       <c r="S61" s="19"/>
       <c r="T61" s="19"/>
     </row>
-    <row r="62" spans="1:20">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A62" s="13">
         <v>52</v>
       </c>
@@ -3138,7 +3128,7 @@
       <c r="S62" s="19"/>
       <c r="T62" s="19"/>
     </row>
-    <row r="63" spans="1:20">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A63" s="13">
         <v>53</v>
       </c>
@@ -3162,7 +3152,7 @@
       <c r="S63" s="19"/>
       <c r="T63" s="19"/>
     </row>
-    <row r="64" spans="1:20">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A64" s="13">
         <v>54</v>
       </c>
@@ -3186,7 +3176,7 @@
       <c r="S64" s="19"/>
       <c r="T64" s="19"/>
     </row>
-    <row r="65" spans="1:20">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A65" s="13">
         <v>55</v>
       </c>
@@ -3210,7 +3200,7 @@
       <c r="S65" s="19"/>
       <c r="T65" s="19"/>
     </row>
-    <row r="66" spans="1:20">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A66" s="13">
         <v>56</v>
       </c>
@@ -3234,7 +3224,7 @@
       <c r="S66" s="19"/>
       <c r="T66" s="19"/>
     </row>
-    <row r="67" spans="1:20">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A67" s="13">
         <v>57</v>
       </c>
@@ -3258,7 +3248,7 @@
       <c r="S67" s="19"/>
       <c r="T67" s="19"/>
     </row>
-    <row r="68" spans="1:20">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A68" s="13">
         <v>58</v>
       </c>
@@ -3282,7 +3272,7 @@
       <c r="S68" s="19"/>
       <c r="T68" s="19"/>
     </row>
-    <row r="69" spans="1:20">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A69" s="13">
         <v>59</v>
       </c>
@@ -3306,7 +3296,7 @@
       <c r="S69" s="19"/>
       <c r="T69" s="19"/>
     </row>
-    <row r="70" spans="1:20">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A70" s="13">
         <v>60</v>
       </c>
@@ -3330,7 +3320,7 @@
       <c r="S70" s="19"/>
       <c r="T70" s="19"/>
     </row>
-    <row r="71" spans="1:20">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A71" s="13">
         <v>61</v>
       </c>
@@ -3354,7 +3344,7 @@
       <c r="S71" s="19"/>
       <c r="T71" s="19"/>
     </row>
-    <row r="72" spans="1:20">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A72" s="13">
         <v>62</v>
       </c>
@@ -3378,7 +3368,7 @@
       <c r="S72" s="19"/>
       <c r="T72" s="19"/>
     </row>
-    <row r="73" spans="1:20">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A73" s="13">
         <v>63</v>
       </c>
@@ -3402,7 +3392,7 @@
       <c r="S73" s="19"/>
       <c r="T73" s="19"/>
     </row>
-    <row r="74" spans="1:20">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A74" s="13">
         <v>64</v>
       </c>
@@ -3426,7 +3416,7 @@
       <c r="S74" s="19"/>
       <c r="T74" s="19"/>
     </row>
-    <row r="75" spans="1:20">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A75" s="13">
         <v>65</v>
       </c>
@@ -3450,7 +3440,7 @@
       <c r="S75" s="19"/>
       <c r="T75" s="19"/>
     </row>
-    <row r="76" spans="1:20">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A76" s="13">
         <v>66</v>
       </c>
@@ -3474,7 +3464,7 @@
       <c r="S76" s="19"/>
       <c r="T76" s="19"/>
     </row>
-    <row r="77" spans="1:20">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A77" s="13">
         <v>67</v>
       </c>
@@ -3498,7 +3488,7 @@
       <c r="S77" s="19"/>
       <c r="T77" s="19"/>
     </row>
-    <row r="78" spans="1:20">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A78" s="13">
         <v>68</v>
       </c>
@@ -3522,7 +3512,7 @@
       <c r="S78" s="19"/>
       <c r="T78" s="19"/>
     </row>
-    <row r="79" spans="1:20">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A79" s="13">
         <v>69</v>
       </c>
@@ -3546,7 +3536,7 @@
       <c r="S79" s="19"/>
       <c r="T79" s="19"/>
     </row>
-    <row r="80" spans="1:20">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A80" s="13">
         <v>70</v>
       </c>
@@ -3570,7 +3560,7 @@
       <c r="S80" s="19"/>
       <c r="T80" s="19"/>
     </row>
-    <row r="81" spans="1:20">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A81" s="13">
         <v>71</v>
       </c>
@@ -3594,7 +3584,7 @@
       <c r="S81" s="19"/>
       <c r="T81" s="19"/>
     </row>
-    <row r="82" spans="1:20">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A82" s="13">
         <v>72</v>
       </c>
@@ -3618,7 +3608,7 @@
       <c r="S82" s="19"/>
       <c r="T82" s="19"/>
     </row>
-    <row r="83" spans="1:20">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A83" s="13">
         <v>73</v>
       </c>
@@ -3642,7 +3632,7 @@
       <c r="S83" s="19"/>
       <c r="T83" s="19"/>
     </row>
-    <row r="84" spans="1:20">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A84" s="13">
         <v>74</v>
       </c>
@@ -3666,7 +3656,7 @@
       <c r="S84" s="19"/>
       <c r="T84" s="19"/>
     </row>
-    <row r="85" spans="1:20">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A85" s="13">
         <v>75</v>
       </c>
@@ -3690,7 +3680,7 @@
       <c r="S85" s="19"/>
       <c r="T85" s="19"/>
     </row>
-    <row r="86" spans="1:20">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A86" s="13">
         <v>76</v>
       </c>
@@ -3714,7 +3704,7 @@
       <c r="S86" s="19"/>
       <c r="T86" s="19"/>
     </row>
-    <row r="87" spans="1:20">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A87" s="13">
         <v>77</v>
       </c>
@@ -3738,7 +3728,7 @@
       <c r="S87" s="19"/>
       <c r="T87" s="19"/>
     </row>
-    <row r="88" spans="1:20">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A88" s="13">
         <v>78</v>
       </c>
@@ -3762,7 +3752,7 @@
       <c r="S88" s="19"/>
       <c r="T88" s="19"/>
     </row>
-    <row r="89" spans="1:20">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A89" s="13">
         <v>79</v>
       </c>
@@ -3786,7 +3776,7 @@
       <c r="S89" s="19"/>
       <c r="T89" s="19"/>
     </row>
-    <row r="90" spans="1:20">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A90" s="13">
         <v>80</v>
       </c>
@@ -3810,7 +3800,7 @@
       <c r="S90" s="19"/>
       <c r="T90" s="19"/>
     </row>
-    <row r="91" spans="1:20">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A91" s="13">
         <v>81</v>
       </c>
@@ -3834,7 +3824,7 @@
       <c r="S91" s="19"/>
       <c r="T91" s="19"/>
     </row>
-    <row r="92" spans="1:20">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A92" s="13">
         <v>82</v>
       </c>
@@ -3858,7 +3848,7 @@
       <c r="S92" s="19"/>
       <c r="T92" s="19"/>
     </row>
-    <row r="93" spans="1:20">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A93" s="13">
         <v>83</v>
       </c>
@@ -3882,7 +3872,7 @@
       <c r="S93" s="19"/>
       <c r="T93" s="19"/>
     </row>
-    <row r="94" spans="1:20">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A94" s="13">
         <v>84</v>
       </c>
@@ -3906,7 +3896,7 @@
       <c r="S94" s="19"/>
       <c r="T94" s="19"/>
     </row>
-    <row r="95" spans="1:20">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A95" s="13">
         <v>85</v>
       </c>
@@ -3930,7 +3920,7 @@
       <c r="S95" s="19"/>
       <c r="T95" s="19"/>
     </row>
-    <row r="96" spans="1:20">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A96" s="13">
         <v>86</v>
       </c>
@@ -3954,7 +3944,7 @@
       <c r="S96" s="19"/>
       <c r="T96" s="19"/>
     </row>
-    <row r="97" spans="1:20">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A97" s="13">
         <v>87</v>
       </c>
@@ -3978,7 +3968,7 @@
       <c r="S97" s="19"/>
       <c r="T97" s="19"/>
     </row>
-    <row r="98" spans="1:20">
+    <row r="98" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A98" s="13">
         <v>88</v>
       </c>
@@ -4002,7 +3992,7 @@
       <c r="S98" s="19"/>
       <c r="T98" s="19"/>
     </row>
-    <row r="99" spans="1:20">
+    <row r="99" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A99" s="13">
         <v>89</v>
       </c>
@@ -4026,7 +4016,7 @@
       <c r="S99" s="19"/>
       <c r="T99" s="19"/>
     </row>
-    <row r="100" spans="1:20">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A100" s="13">
         <v>90</v>
       </c>
@@ -4050,7 +4040,7 @@
       <c r="S100" s="19"/>
       <c r="T100" s="19"/>
     </row>
-    <row r="101" spans="1:20">
+    <row r="101" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A101" s="13">
         <v>91</v>
       </c>
@@ -4074,7 +4064,7 @@
       <c r="S101" s="19"/>
       <c r="T101" s="19"/>
     </row>
-    <row r="102" spans="1:20">
+    <row r="102" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A102" s="13">
         <v>92</v>
       </c>
@@ -4098,7 +4088,7 @@
       <c r="S102" s="19"/>
       <c r="T102" s="19"/>
     </row>
-    <row r="103" spans="1:20">
+    <row r="103" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A103" s="13">
         <v>93</v>
       </c>
@@ -4122,7 +4112,7 @@
       <c r="S103" s="19"/>
       <c r="T103" s="19"/>
     </row>
-    <row r="104" spans="1:20">
+    <row r="104" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A104" s="13">
         <v>94</v>
       </c>
@@ -4146,7 +4136,7 @@
       <c r="S104" s="19"/>
       <c r="T104" s="19"/>
     </row>
-    <row r="105" spans="1:20">
+    <row r="105" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A105" s="13">
         <v>95</v>
       </c>
@@ -4170,7 +4160,7 @@
       <c r="S105" s="19"/>
       <c r="T105" s="19"/>
     </row>
-    <row r="106" spans="1:20">
+    <row r="106" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A106" s="13">
         <v>96</v>
       </c>
@@ -4194,7 +4184,7 @@
       <c r="S106" s="19"/>
       <c r="T106" s="19"/>
     </row>
-    <row r="107" spans="1:20">
+    <row r="107" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A107" s="13">
         <v>97</v>
       </c>
@@ -4218,7 +4208,7 @@
       <c r="S107" s="19"/>
       <c r="T107" s="19"/>
     </row>
-    <row r="108" spans="1:20">
+    <row r="108" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A108" s="13">
         <v>98</v>
       </c>
@@ -4242,7 +4232,7 @@
       <c r="S108" s="19"/>
       <c r="T108" s="19"/>
     </row>
-    <row r="109" spans="1:20">
+    <row r="109" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A109" s="13">
         <v>99</v>
       </c>
@@ -4266,7 +4256,7 @@
       <c r="S109" s="19"/>
       <c r="T109" s="19"/>
     </row>
-    <row r="110" spans="1:20">
+    <row r="110" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A110" s="13">
         <v>100</v>
       </c>
@@ -4290,7 +4280,7 @@
       <c r="S110" s="19"/>
       <c r="T110" s="19"/>
     </row>
-    <row r="111" spans="1:20">
+    <row r="111" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B111" s="19"/>
       <c r="C111" s="19"/>
       <c r="D111" s="19"/>
@@ -4311,7 +4301,7 @@
       <c r="S111" s="19"/>
       <c r="T111" s="19"/>
     </row>
-    <row r="112" spans="1:20">
+    <row r="112" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B112" s="19"/>
       <c r="C112" s="19"/>
       <c r="D112" s="19"/>
@@ -4332,7 +4322,7 @@
       <c r="S112" s="19"/>
       <c r="T112" s="19"/>
     </row>
-    <row r="113" spans="2:20">
+    <row r="113" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B113" s="19"/>
       <c r="C113" s="19"/>
       <c r="D113" s="19"/>
@@ -4353,7 +4343,7 @@
       <c r="S113" s="19"/>
       <c r="T113" s="19"/>
     </row>
-    <row r="114" spans="2:20">
+    <row r="114" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B114" s="19"/>
       <c r="C114" s="19"/>
       <c r="D114" s="19"/>
@@ -4374,7 +4364,7 @@
       <c r="S114" s="19"/>
       <c r="T114" s="19"/>
     </row>
-    <row r="115" spans="2:20">
+    <row r="115" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B115" s="19"/>
       <c r="C115" s="19"/>
       <c r="D115" s="19"/>
@@ -4395,7 +4385,7 @@
       <c r="S115" s="19"/>
       <c r="T115" s="19"/>
     </row>
-    <row r="116" spans="2:20">
+    <row r="116" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B116" s="19"/>
       <c r="C116" s="19"/>
       <c r="D116" s="19"/>
@@ -4416,7 +4406,7 @@
       <c r="S116" s="19"/>
       <c r="T116" s="19"/>
     </row>
-    <row r="117" spans="2:20">
+    <row r="117" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B117" s="19"/>
       <c r="C117" s="19"/>
       <c r="D117" s="19"/>
@@ -4437,7 +4427,7 @@
       <c r="S117" s="19"/>
       <c r="T117" s="19"/>
     </row>
-    <row r="118" spans="2:20">
+    <row r="118" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B118" s="19"/>
       <c r="C118" s="19"/>
       <c r="D118" s="19"/>
@@ -4458,7 +4448,7 @@
       <c r="S118" s="19"/>
       <c r="T118" s="19"/>
     </row>
-    <row r="119" spans="2:20">
+    <row r="119" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B119" s="19"/>
       <c r="C119" s="19"/>
       <c r="D119" s="19"/>
@@ -4479,7 +4469,7 @@
       <c r="S119" s="19"/>
       <c r="T119" s="19"/>
     </row>
-    <row r="120" spans="2:20">
+    <row r="120" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B120" s="19"/>
       <c r="C120" s="19"/>
       <c r="D120" s="19"/>
@@ -4500,7 +4490,7 @@
       <c r="S120" s="19"/>
       <c r="T120" s="19"/>
     </row>
-    <row r="121" spans="2:20">
+    <row r="121" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B121" s="19"/>
       <c r="C121" s="19"/>
       <c r="D121" s="19"/>
@@ -4521,7 +4511,7 @@
       <c r="S121" s="19"/>
       <c r="T121" s="19"/>
     </row>
-    <row r="122" spans="2:20">
+    <row r="122" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B122" s="19"/>
       <c r="C122" s="19"/>
       <c r="D122" s="19"/>
@@ -4542,7 +4532,7 @@
       <c r="S122" s="19"/>
       <c r="T122" s="19"/>
     </row>
-    <row r="123" spans="2:20">
+    <row r="123" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B123" s="19"/>
       <c r="C123" s="19"/>
       <c r="D123" s="19"/>
@@ -4563,7 +4553,7 @@
       <c r="S123" s="19"/>
       <c r="T123" s="19"/>
     </row>
-    <row r="124" spans="2:20">
+    <row r="124" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B124" s="19"/>
       <c r="C124" s="19"/>
       <c r="D124" s="19"/>
@@ -4584,7 +4574,7 @@
       <c r="S124" s="19"/>
       <c r="T124" s="19"/>
     </row>
-    <row r="125" spans="2:20">
+    <row r="125" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B125" s="19"/>
       <c r="C125" s="19"/>
       <c r="D125" s="19"/>
@@ -4605,7 +4595,7 @@
       <c r="S125" s="19"/>
       <c r="T125" s="19"/>
     </row>
-    <row r="126" spans="2:20">
+    <row r="126" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B126" s="19"/>
       <c r="C126" s="19"/>
       <c r="D126" s="19"/>
@@ -4626,7 +4616,7 @@
       <c r="S126" s="19"/>
       <c r="T126" s="19"/>
     </row>
-    <row r="127" spans="2:20">
+    <row r="127" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B127" s="19"/>
       <c r="C127" s="19"/>
       <c r="D127" s="19"/>
@@ -4647,7 +4637,7 @@
       <c r="S127" s="19"/>
       <c r="T127" s="19"/>
     </row>
-    <row r="128" spans="2:20">
+    <row r="128" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B128" s="19"/>
       <c r="C128" s="19"/>
       <c r="D128" s="19"/>
@@ -4668,7 +4658,7 @@
       <c r="S128" s="19"/>
       <c r="T128" s="19"/>
     </row>
-    <row r="129" spans="2:20">
+    <row r="129" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B129" s="19"/>
       <c r="C129" s="19"/>
       <c r="D129" s="19"/>
@@ -4689,7 +4679,7 @@
       <c r="S129" s="19"/>
       <c r="T129" s="19"/>
     </row>
-    <row r="130" spans="2:20">
+    <row r="130" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B130" s="19"/>
       <c r="C130" s="19"/>
       <c r="D130" s="19"/>
@@ -4710,7 +4700,7 @@
       <c r="S130" s="19"/>
       <c r="T130" s="19"/>
     </row>
-    <row r="131" spans="2:20">
+    <row r="131" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B131" s="19"/>
       <c r="C131" s="19"/>
       <c r="D131" s="19"/>
@@ -4731,7 +4721,7 @@
       <c r="S131" s="19"/>
       <c r="T131" s="19"/>
     </row>
-    <row r="132" spans="2:20">
+    <row r="132" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B132" s="19"/>
       <c r="C132" s="19"/>
       <c r="D132" s="19"/>
@@ -4752,7 +4742,7 @@
       <c r="S132" s="19"/>
       <c r="T132" s="19"/>
     </row>
-    <row r="133" spans="2:20">
+    <row r="133" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B133" s="19"/>
       <c r="C133" s="19"/>
       <c r="D133" s="19"/>
@@ -4773,7 +4763,7 @@
       <c r="S133" s="19"/>
       <c r="T133" s="19"/>
     </row>
-    <row r="134" spans="2:20">
+    <row r="134" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B134" s="19"/>
       <c r="C134" s="19"/>
       <c r="D134" s="19"/>
@@ -4794,7 +4784,7 @@
       <c r="S134" s="19"/>
       <c r="T134" s="19"/>
     </row>
-    <row r="135" spans="2:20">
+    <row r="135" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B135" s="19"/>
       <c r="C135" s="19"/>
       <c r="D135" s="19"/>
@@ -4815,7 +4805,7 @@
       <c r="S135" s="19"/>
       <c r="T135" s="19"/>
     </row>
-    <row r="136" spans="2:20">
+    <row r="136" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B136" s="19"/>
       <c r="C136" s="19"/>
       <c r="D136" s="19"/>
@@ -4836,7 +4826,7 @@
       <c r="S136" s="19"/>
       <c r="T136" s="19"/>
     </row>
-    <row r="137" spans="2:20">
+    <row r="137" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B137" s="19"/>
       <c r="C137" s="19"/>
       <c r="D137" s="19"/>
@@ -4857,7 +4847,7 @@
       <c r="S137" s="19"/>
       <c r="T137" s="19"/>
     </row>
-    <row r="138" spans="2:20">
+    <row r="138" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B138" s="19"/>
       <c r="C138" s="19"/>
       <c r="D138" s="19"/>
@@ -4878,7 +4868,7 @@
       <c r="S138" s="19"/>
       <c r="T138" s="19"/>
     </row>
-    <row r="139" spans="2:20">
+    <row r="139" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B139" s="19"/>
       <c r="C139" s="19"/>
       <c r="D139" s="19"/>
@@ -4899,7 +4889,7 @@
       <c r="S139" s="19"/>
       <c r="T139" s="19"/>
     </row>
-    <row r="140" spans="2:20">
+    <row r="140" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B140" s="19"/>
       <c r="C140" s="19"/>
       <c r="D140" s="19"/>

</xml_diff>